<commit_message>
Update Cylindrical Roller Bearings.xlsx
</commit_message>
<xml_diff>
--- a/Cylindrical Roller Bearings.xlsx
+++ b/Cylindrical Roller Bearings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlanticbearing-my.sharepoint.com/personal/rishi_sivakumar_atlantic-bearing_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlanticbearing-my.sharepoint.com/personal/rishi_sivakumar_atlantic-bearing_com/Documents/Documents/GitHub/BearingManualAutomation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="703" documentId="8_{D50A434F-5045-4162-B3DF-0316DFB4F095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20069380-5FA3-4E19-A66E-A1B7F916CEBA}"/>
+  <xr:revisionPtr revIDLastSave="706" documentId="8_{D50A434F-5045-4162-B3DF-0316DFB4F095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F7949D5-A5DA-458B-B9F9-858C302E5E28}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{72A27418-34D0-4484-85A3-F3570DFD4D7B}"/>
   </bookViews>
@@ -38,15 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>1 180</t>
   </si>
   <si>
@@ -57,6 +48,15 @@
   </si>
   <si>
     <t>r34</t>
+  </si>
+  <si>
+    <t>inner_diameter</t>
+  </si>
+  <si>
+    <t>outer diameter</t>
+  </si>
+  <si>
+    <t>width</t>
   </si>
 </sst>
 </file>
@@ -113,12 +113,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +456,7 @@
   <dimension ref="A1:F556"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -468,22 +468,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
@@ -11531,7 +11531,7 @@
         <v>900</v>
       </c>
       <c r="B554" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C554" s="3">
         <v>165</v>

</xml_diff>